<commit_message>
In testing had modified and saved in order to verify test failure if downloaded file did not match master. Changed back and saved.
Updated comments
</commit_message>
<xml_diff>
--- a/SightlyTestProject/ComparisonFiles/PerformanceDetail-AdWords-Ad_Group_Mapping-Master.xlsx
+++ b/SightlyTestProject/ComparisonFiles/PerformanceDetail-AdWords-Ad_Group_Mapping-Master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.hamilton\source\repos\SightlyTestProject\SightlyTestProject\ComparisonFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.hamilton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8A33B8-E6A5-490E-94AC-E981BBA04F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA810F1F-29D4-4FAC-ACD8-C90839B09A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17244" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31230" yWindow="3210" windowWidth="17250" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance Detail" sheetId="1" r:id="rId1"/>

</xml_diff>